<commit_message>
household controls for non-GQ only
</commit_message>
<xml_diff>
--- a/models/populationsim-taz/data-dictionary.xlsx
+++ b/models/populationsim-taz/data-dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/Link21-TLDU/models/populationsim-taz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8FFF47-F1CD-5B41-8A1E-B446E5A24EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3D6167-97B4-5C49-9349-5BF879525537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{91DB2D60-C73A-2645-8909-4988E2748C3C}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>Production, transportation, and material moving</t>
   </si>
   <si>
-    <t>hh_workers_from_esr</t>
-  </si>
-  <si>
     <t>Household workers, which is sum of `employed`</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>Any variable expressed in CAPs not included in this table is from PUMS; see PUMS data dictionary</t>
   </si>
   <si>
-    <t>HHINC</t>
-  </si>
-  <si>
     <t>Same as `hh_income_2000`</t>
   </si>
   <si>
@@ -224,6 +218,12 @@
   </si>
   <si>
     <t>Whether the person is employed (ESR == 1, 2, 4, or 5)</t>
+  </si>
+  <si>
+    <t>HINC</t>
+  </si>
+  <si>
+    <t>hworkers</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -636,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -658,7 +658,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1148,10 +1148,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>33</v>
@@ -1165,10 +1165,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>33</v>
@@ -1182,16 +1182,16 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1199,10 +1199,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>33</v>
@@ -1216,10 +1216,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>33</v>
@@ -1233,10 +1233,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>33</v>
@@ -1250,10 +1250,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>33</v>
@@ -1267,10 +1267,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>33</v>

</xml_diff>